<commit_message>
hertrainen na elke stap werkt. Format van output fixen.
</commit_message>
<xml_diff>
--- a/PCAcombined_predicted_factors_matrix_10.xlsx
+++ b/PCAcombined_predicted_factors_matrix_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,31 +440,13 @@
       <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>0.1321849163323346</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2027588370709348</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.123443710001759</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.05721559677157786</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.009614008363069554</v>
+        <v>0.2027848664202113</v>
       </c>
     </row>
     <row r="3">
@@ -472,16 +454,7 @@
         <v>0.2491991661712655</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1724190039994039</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1027944390189974</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.06160873912032113</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.04407524810461526</v>
+        <v>0.1724411384451406</v>
       </c>
     </row>
     <row r="4">
@@ -489,16 +462,7 @@
         <v>0.977151395024658</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.6742682762825989</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-0.3423737996741228</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.2000048012873049</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-0.1258392457337382</v>
+        <v>-0.6743548360830079</v>
       </c>
     </row>
     <row r="5">
@@ -506,16 +470,7 @@
         <v>0.5172165385330864</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3121925462620068</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.1686536152481463</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.08583553160390504</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.04075965296671515</v>
+        <v>0.3122326242627769</v>
       </c>
     </row>
     <row r="6">
@@ -523,16 +478,7 @@
         <v>-0.5865045841730135</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.2698073218999459</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-0.03339032416121902</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.009953462608685626</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.01806342261183984</v>
+        <v>-0.2698419586591628</v>
       </c>
     </row>
     <row r="7">
@@ -540,16 +486,7 @@
         <v>0.1420548882957302</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1153313403414525</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.03774514565473479</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.007610161520114371</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-0.003788177753993734</v>
+        <v>0.1153461461066831</v>
       </c>
     </row>
     <row r="8">
@@ -557,16 +494,7 @@
         <v>0.01645775632661547</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01276403428592806</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.06652909409328379</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.04107371382211161</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.01955116310837636</v>
+        <v>0.01276567288038519</v>
       </c>
     </row>
     <row r="9">
@@ -574,16 +502,7 @@
         <v>0.2430084726874119</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1178431363494902</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.03075833393271684</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.004062916759965143</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-0.006709771309508726</v>
+        <v>0.1178582645688076</v>
       </c>
     </row>
     <row r="10">
@@ -591,16 +510,7 @@
         <v>-0.02063914468007719</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.005733852211510635</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-0.003624164128976591</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.007797663775166226</v>
-      </c>
-      <c r="E10" t="n">
-        <v>-0.006608080888091944</v>
+        <v>-0.005734588299979596</v>
       </c>
     </row>
     <row r="11">
@@ -608,16 +518,7 @@
         <v>-0.1152244858542527</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.02648602223019105</v>
-      </c>
-      <c r="C11" t="n">
-        <v>-0.01844045203851006</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-0.007076208906844147</v>
-      </c>
-      <c r="E11" t="n">
-        <v>-0.002667546678723493</v>
+        <v>-0.02648942239727368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>